<commit_message>
Adição da US16 ao Backlog da segunda sprint
</commit_message>
<xml_diff>
--- a/product-backlog/Product Backlog Segunda Sprint.xlsx
+++ b/product-backlog/Product Backlog Segunda Sprint.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25721"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vitao\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Carlos Gênio\AppData\Roaming\Microsoft\Windows\Network Shortcuts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6F3C2CF-0239-4253-A5FB-9B9F8FD0177F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{C8077C63-64F8-4271-9CA2-AA38E5376211}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{0463CAB5-11B3-42C2-8D94-09BE11B1B912}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="2" xr2:uid="{0463CAB5-11B3-42C2-8D94-09BE11B1B912}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sprint 1 - Backlog" sheetId="2" r:id="rId1"/>
-    <sheet name="Sprint 2 - Backlog" sheetId="3" r:id="rId2"/>
+    <sheet name="Product Backlog" sheetId="1" r:id="rId1"/>
+    <sheet name="Sprint 1 - Backlog" sheetId="2" r:id="rId2"/>
+    <sheet name="Sprint 2 - Backlog" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="115">
   <si>
     <t>Product Backlog</t>
   </si>
@@ -136,6 +137,9 @@
     <t>Preencher o valor de saque desejado.</t>
   </si>
   <si>
+    <t>Se o valor estiver de acordo derá exibir mensagem de "Saque Realizado"; Caso o valor seja maior que a quantia que o banco tem disponivel, mostrar mensagem ''Empréstimo Negado''.</t>
+  </si>
+  <si>
     <t>US05</t>
   </si>
   <si>
@@ -288,14 +292,110 @@
     <t>Se usuário logado o mesmo poderá acessar a tela de extrato.Caso contrário o usuário será direcionado para a tela de login para validação de acesso</t>
   </si>
   <si>
+    <t>US16</t>
+  </si>
+  <si>
+    <t>Eu, enquanto usuário comum, desejo acompanhar minha solicitação de abertura de conta para após confirmado saber minha agência e conta</t>
+  </si>
+  <si>
+    <t>O usuário deverá preencher com o CPF e senha e clicar no botão "Acompanhar abertura de conta"</t>
+  </si>
+  <si>
+    <t>Se os dados forem prenchidos corretamente e a solicitação de abertura for aprovada, a agência e conta será mostrada na tela. Caso contrário, uma mensagem dizendo que a solicitação está em analise será mostrada.</t>
+  </si>
+  <si>
+    <t>Eu, enquanto usuário, desejo acessar tela de dados cadastrais, para solicitar alterações dos dados.</t>
+  </si>
+  <si>
+    <t>EU, enquanto gerente de agência, desejo ter acesso a tela de edição de dados cadastrais de usuário, para atender solicitações do usuário.</t>
+  </si>
+  <si>
+    <t>EU, enquanto usuário, desejo acessar a tela de encerramento, para encerrar minha conta no banco.</t>
+  </si>
+  <si>
+    <t>EU, enquanto gerente de agência, desejo ter acesso a tela de encerramento de conta, para validar solicitação de encerramento de contas de usuário comum.</t>
+  </si>
+  <si>
+    <t>Eu enquanto desenvolvedor desejo criar tela de transferência, para que o usuário possa realizar transferências.</t>
+  </si>
+  <si>
+    <t>US17</t>
+  </si>
+  <si>
+    <t>Eu, enquanto usuário desejo, acessar a tela de transferência para realizar transferências.</t>
+  </si>
+  <si>
+    <t>US18</t>
+  </si>
+  <si>
+    <t>Eu, enquanto gerente de agência desejo acessar a tela administrativa para aceitar as solicitações</t>
+  </si>
+  <si>
+    <t>US19</t>
+  </si>
+  <si>
+    <t>EU, enquanto desenvolvedor, desejo criar a tela administrativa, para atribuir acesso ao gerente geral.</t>
+  </si>
+  <si>
+    <t>US20</t>
+  </si>
+  <si>
+    <t>Eu, enquanto gerente geral, desejo acessar a tela administrativa, para criar agência.</t>
+  </si>
+  <si>
+    <t>US21</t>
+  </si>
+  <si>
+    <t>Eu, enquanto gerente geral, desejo acessar a tela administrativa, para criar cadastro de gerente de agência.</t>
+  </si>
+  <si>
+    <t>US22</t>
+  </si>
+  <si>
+    <t>Eu, enquanto gerente geral, desejo acessar a tela administrativa, para validar abertura de conta do gerente de agência.</t>
+  </si>
+  <si>
+    <t>US23</t>
+  </si>
+  <si>
+    <t>Eu, enquanto gerente geral, desejo acessar a tela administrativa, para confirmar abertura de conta de gerente de agência.</t>
+  </si>
+  <si>
+    <t>US24</t>
+  </si>
+  <si>
+    <t>EU, enquanto gerente geral, desejo ter acesso a tela administrativa, para definir o capital inicial do banco.</t>
+  </si>
+  <si>
+    <t>US25</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EU, enquanto gerente geral, desejo ter acesso a tela administrativa,  para configurações de agência e gerente. </t>
+  </si>
+  <si>
+    <t>US26</t>
+  </si>
+  <si>
+    <t>EU, enquanto gerente geral, desejo ter acesso a tela administrativa, para poder alterar as taxas.</t>
+  </si>
+  <si>
     <t>Se o valor estiver de acordo deverá exibir mensagem de "Saque Realizado"; Caso o valor seja maior que a quantia que o banco tem disponivel, mostrar mensagem ''Empréstimo Negado''.</t>
+  </si>
+  <si>
+    <t>Se a tela de confirmação de depósito for visualizada haverá um botão de confirmação da operação. Caso contrário aparecerá a mensagem de efetuar login, ou a mensagem de que o valor deverá ser maior que 0 reais.</t>
+  </si>
+  <si>
+    <t>Se a tela de confirmação de saque for visualizada haverá um botão de confirmação da operação. Caso contrário aparecerá a mensagem de efetuar login, ou a mensagem de que o valor deverá ser maior que 0 reais.</t>
+  </si>
+  <si>
+    <t>Se usuário logado o mesmo poderá acessar a tela de extrato.Caso contrário o usuário será direcionado para a tela de login para validação de acesso.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -339,6 +439,12 @@
       <color theme="1"/>
       <name val="Calibri"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <charset val="1"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -348,7 +454,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="16">
+  <borders count="29">
     <border>
       <left/>
       <right/>
@@ -415,6 +521,21 @@
       <diagonal/>
     </border>
     <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
@@ -434,42 +555,42 @@
         <color rgb="FF000000"/>
       </left>
       <right style="thin">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </right>
-      <top style="medium">
-        <color rgb="FF000000"/>
+      <top style="thin">
+        <color indexed="64"/>
       </top>
-      <bottom style="thin">
+      <bottom style="medium">
         <color rgb="FF000000"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </left>
       <right style="thin">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </right>
-      <top style="medium">
-        <color rgb="FF000000"/>
+      <top style="thin">
+        <color indexed="64"/>
       </top>
-      <bottom style="thin">
+      <bottom style="medium">
         <color rgb="FF000000"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </left>
       <right style="medium">
         <color rgb="FF000000"/>
       </right>
-      <top style="medium">
-        <color rgb="FF000000"/>
+      <top style="thin">
+        <color indexed="64"/>
       </top>
-      <bottom style="thin">
+      <bottom style="medium">
         <color rgb="FF000000"/>
       </bottom>
       <diagonal/>
@@ -479,27 +600,132 @@
         <color rgb="FF000000"/>
       </left>
       <right style="thin">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </right>
-      <top style="thin">
+      <top style="medium">
         <color rgb="FF000000"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
       </left>
       <right style="medium">
         <color rgb="FF000000"/>
       </right>
-      <top style="thin">
+      <top style="medium">
         <color rgb="FF000000"/>
       </top>
       <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
         <color rgb="FF000000"/>
       </bottom>
       <diagonal/>
@@ -568,6 +794,63 @@
         <color rgb="FF000000"/>
       </right>
       <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
         <color rgb="FF000000"/>
       </top>
       <bottom/>
@@ -577,7 +860,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="79">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -630,62 +913,145 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -694,6 +1060,36 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -714,7 +1110,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1009,14 +1405,1002 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7B3495A-186F-4DC8-BB09-521976E4C63A}">
+  <dimension ref="A1:G72"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A21" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26:G33"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="13.42578125" customWidth="1"/>
+    <col min="2" max="2" width="6" customWidth="1"/>
+    <col min="3" max="3" width="24" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="82.28515625" style="6" customWidth="1"/>
+    <col min="5" max="5" width="19.85546875" customWidth="1"/>
+    <col min="6" max="6" width="47.7109375" style="6" customWidth="1"/>
+    <col min="7" max="7" width="32.28515625" style="6" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="46.5">
+      <c r="A1" s="71" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="71"/>
+      <c r="C1" s="71"/>
+      <c r="D1" s="71"/>
+      <c r="E1" s="71"/>
+      <c r="F1" s="71"/>
+      <c r="G1" s="71"/>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" s="30" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="31" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="31" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="32" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="33" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="32" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" s="34" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="76.5">
+      <c r="A3" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="1">
+        <v>1</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" s="25" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="76.5">
+      <c r="A4" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="1">
+        <v>1</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G4" s="25" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="76.5">
+      <c r="A5" s="24" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" s="1">
+        <v>1</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G5" s="25" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="159" customHeight="1">
+      <c r="A6" s="26" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6" s="27">
+        <v>1</v>
+      </c>
+      <c r="C6" s="27" t="s">
+        <v>27</v>
+      </c>
+      <c r="D6" s="28" t="s">
+        <v>28</v>
+      </c>
+      <c r="E6" s="35" t="s">
+        <v>29</v>
+      </c>
+      <c r="F6" s="28" t="s">
+        <v>30</v>
+      </c>
+      <c r="G6" s="29" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="51" customHeight="1">
+      <c r="A7" s="75"/>
+      <c r="B7" s="75"/>
+      <c r="C7" s="75"/>
+      <c r="D7" s="75"/>
+      <c r="E7" s="75"/>
+      <c r="F7" s="75"/>
+      <c r="G7" s="75"/>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" s="76"/>
+      <c r="B8" s="76"/>
+      <c r="C8" s="76"/>
+      <c r="D8" s="76"/>
+      <c r="E8" s="76"/>
+      <c r="F8" s="76"/>
+      <c r="G8" s="76"/>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" s="76"/>
+      <c r="B9" s="76"/>
+      <c r="C9" s="76"/>
+      <c r="D9" s="76"/>
+      <c r="E9" s="76"/>
+      <c r="F9" s="76"/>
+      <c r="G9" s="76"/>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" s="76"/>
+      <c r="B10" s="76"/>
+      <c r="C10" s="76"/>
+      <c r="D10" s="76"/>
+      <c r="E10" s="76"/>
+      <c r="F10" s="76"/>
+      <c r="G10" s="76"/>
+    </row>
+    <row r="11" spans="1:7" ht="38.25" customHeight="1">
+      <c r="A11" s="77"/>
+      <c r="B11" s="77"/>
+      <c r="C11" s="77"/>
+      <c r="D11" s="77"/>
+      <c r="E11" s="77"/>
+      <c r="F11" s="77"/>
+      <c r="G11" s="77"/>
+    </row>
+    <row r="12" spans="1:7" ht="51" customHeight="1">
+      <c r="A12" s="72" t="s">
+        <v>0</v>
+      </c>
+      <c r="B12" s="73"/>
+      <c r="C12" s="73"/>
+      <c r="D12" s="73"/>
+      <c r="E12" s="73"/>
+      <c r="F12" s="73"/>
+      <c r="G12" s="74"/>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13" s="37" t="s">
+        <v>1</v>
+      </c>
+      <c r="B13" s="38" t="s">
+        <v>2</v>
+      </c>
+      <c r="C13" s="38" t="s">
+        <v>3</v>
+      </c>
+      <c r="D13" s="39" t="s">
+        <v>4</v>
+      </c>
+      <c r="E13" s="40" t="s">
+        <v>5</v>
+      </c>
+      <c r="F13" s="39" t="s">
+        <v>6</v>
+      </c>
+      <c r="G13" s="41" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="137.25">
+      <c r="A14" s="42" t="s">
+        <v>32</v>
+      </c>
+      <c r="B14" s="36">
+        <v>2</v>
+      </c>
+      <c r="C14" s="23" t="s">
+        <v>33</v>
+      </c>
+      <c r="D14" s="50" t="s">
+        <v>34</v>
+      </c>
+      <c r="E14" s="54" t="s">
+        <v>11</v>
+      </c>
+      <c r="F14" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="G14" s="44" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="73.5" customHeight="1">
+      <c r="A15" s="42" t="s">
+        <v>37</v>
+      </c>
+      <c r="B15" s="36">
+        <v>2</v>
+      </c>
+      <c r="C15" s="23" t="s">
+        <v>38</v>
+      </c>
+      <c r="D15" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="E15" s="54" t="s">
+        <v>40</v>
+      </c>
+      <c r="F15" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="G15" s="44" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="126" customHeight="1">
+      <c r="A16" s="42" t="s">
+        <v>43</v>
+      </c>
+      <c r="B16" s="36">
+        <v>2</v>
+      </c>
+      <c r="C16" s="23" t="s">
+        <v>44</v>
+      </c>
+      <c r="D16" s="21" t="s">
+        <v>45</v>
+      </c>
+      <c r="E16" s="54" t="s">
+        <v>46</v>
+      </c>
+      <c r="F16" s="21" t="s">
+        <v>47</v>
+      </c>
+      <c r="G16" s="44" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="126" customHeight="1">
+      <c r="A17" s="42" t="s">
+        <v>49</v>
+      </c>
+      <c r="B17" s="36"/>
+      <c r="C17" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="E17" s="54" t="s">
+        <v>51</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G17" s="25" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="126" customHeight="1">
+      <c r="A18" s="42" t="s">
+        <v>52</v>
+      </c>
+      <c r="B18" s="36"/>
+      <c r="C18" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="E18" s="54" t="s">
+        <v>51</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="G18" s="25" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="106.5">
+      <c r="A19" s="42" t="s">
+        <v>56</v>
+      </c>
+      <c r="B19" s="36">
+        <v>2</v>
+      </c>
+      <c r="C19" s="23" t="s">
+        <v>44</v>
+      </c>
+      <c r="D19" s="21" t="s">
+        <v>57</v>
+      </c>
+      <c r="E19" s="54" t="s">
+        <v>46</v>
+      </c>
+      <c r="F19" s="21" t="s">
+        <v>58</v>
+      </c>
+      <c r="G19" s="44" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="106.5">
+      <c r="A20" s="42" t="s">
+        <v>60</v>
+      </c>
+      <c r="B20" s="36">
+        <v>2</v>
+      </c>
+      <c r="C20" s="23" t="s">
+        <v>44</v>
+      </c>
+      <c r="D20" s="21" t="s">
+        <v>61</v>
+      </c>
+      <c r="E20" s="54" t="s">
+        <v>62</v>
+      </c>
+      <c r="F20" s="21" t="s">
+        <v>63</v>
+      </c>
+      <c r="G20" s="44" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="106.5">
+      <c r="A21" s="42" t="s">
+        <v>65</v>
+      </c>
+      <c r="B21" s="36">
+        <v>2</v>
+      </c>
+      <c r="C21" s="23" t="s">
+        <v>44</v>
+      </c>
+      <c r="D21" s="21" t="s">
+        <v>66</v>
+      </c>
+      <c r="E21" s="54" t="s">
+        <v>62</v>
+      </c>
+      <c r="F21" s="21" t="s">
+        <v>67</v>
+      </c>
+      <c r="G21" s="44" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="78" customHeight="1">
+      <c r="A22" s="42" t="s">
+        <v>69</v>
+      </c>
+      <c r="B22" s="36">
+        <v>2</v>
+      </c>
+      <c r="C22" s="23" t="s">
+        <v>44</v>
+      </c>
+      <c r="D22" s="21" t="s">
+        <v>70</v>
+      </c>
+      <c r="E22" s="54" t="s">
+        <v>23</v>
+      </c>
+      <c r="F22" s="21" t="s">
+        <v>71</v>
+      </c>
+      <c r="G22" s="44" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="75.75" customHeight="1">
+      <c r="A23" s="42" t="s">
+        <v>73</v>
+      </c>
+      <c r="B23" s="36">
+        <v>2</v>
+      </c>
+      <c r="C23" s="23" t="s">
+        <v>44</v>
+      </c>
+      <c r="D23" s="21" t="s">
+        <v>74</v>
+      </c>
+      <c r="E23" s="54" t="s">
+        <v>23</v>
+      </c>
+      <c r="F23" s="21" t="s">
+        <v>75</v>
+      </c>
+      <c r="G23" s="44" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="76.5">
+      <c r="A24" s="42" t="s">
+        <v>76</v>
+      </c>
+      <c r="B24" s="46">
+        <v>2</v>
+      </c>
+      <c r="C24" s="23" t="s">
+        <v>77</v>
+      </c>
+      <c r="D24" s="58" t="s">
+        <v>78</v>
+      </c>
+      <c r="E24" s="54" t="s">
+        <v>79</v>
+      </c>
+      <c r="F24" s="58" t="s">
+        <v>80</v>
+      </c>
+      <c r="G24" s="49" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="106.5">
+      <c r="A25" s="42" t="s">
+        <v>82</v>
+      </c>
+      <c r="B25" s="46">
+        <v>2</v>
+      </c>
+      <c r="C25" s="57"/>
+      <c r="D25" s="65" t="s">
+        <v>83</v>
+      </c>
+      <c r="E25" s="64" t="s">
+        <v>51</v>
+      </c>
+      <c r="F25" s="58" t="s">
+        <v>84</v>
+      </c>
+      <c r="G25" s="49" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7">
+      <c r="A26" s="76"/>
+      <c r="B26" s="76"/>
+      <c r="C26" s="76"/>
+      <c r="D26" s="76"/>
+      <c r="E26" s="76"/>
+      <c r="F26" s="76"/>
+      <c r="G26" s="76"/>
+    </row>
+    <row r="27" spans="1:7">
+      <c r="A27" s="76"/>
+      <c r="B27" s="76"/>
+      <c r="C27" s="76"/>
+      <c r="D27" s="76"/>
+      <c r="E27" s="76"/>
+      <c r="F27" s="76"/>
+      <c r="G27" s="76"/>
+    </row>
+    <row r="28" spans="1:7">
+      <c r="A28" s="76"/>
+      <c r="B28" s="76"/>
+      <c r="C28" s="76"/>
+      <c r="D28" s="76"/>
+      <c r="E28" s="76"/>
+      <c r="F28" s="76"/>
+      <c r="G28" s="76"/>
+    </row>
+    <row r="29" spans="1:7">
+      <c r="A29" s="76"/>
+      <c r="B29" s="76"/>
+      <c r="C29" s="76"/>
+      <c r="D29" s="76"/>
+      <c r="E29" s="76"/>
+      <c r="F29" s="76"/>
+      <c r="G29" s="76"/>
+    </row>
+    <row r="30" spans="1:7">
+      <c r="A30" s="76"/>
+      <c r="B30" s="76"/>
+      <c r="C30" s="76"/>
+      <c r="D30" s="76"/>
+      <c r="E30" s="76"/>
+      <c r="F30" s="76"/>
+      <c r="G30" s="76"/>
+    </row>
+    <row r="31" spans="1:7">
+      <c r="A31" s="76"/>
+      <c r="B31" s="76"/>
+      <c r="C31" s="76"/>
+      <c r="D31" s="76"/>
+      <c r="E31" s="76"/>
+      <c r="F31" s="76"/>
+      <c r="G31" s="76"/>
+    </row>
+    <row r="32" spans="1:7">
+      <c r="A32" s="76"/>
+      <c r="B32" s="76"/>
+      <c r="C32" s="76"/>
+      <c r="D32" s="76"/>
+      <c r="E32" s="76"/>
+      <c r="F32" s="76"/>
+      <c r="G32" s="76"/>
+    </row>
+    <row r="33" spans="1:7">
+      <c r="A33" s="77"/>
+      <c r="B33" s="77"/>
+      <c r="C33" s="77"/>
+      <c r="D33" s="77"/>
+      <c r="E33" s="77"/>
+      <c r="F33" s="77"/>
+      <c r="G33" s="77"/>
+    </row>
+    <row r="34" spans="1:7" ht="46.5">
+      <c r="A34" s="66" t="s">
+        <v>0</v>
+      </c>
+      <c r="B34" s="67"/>
+      <c r="C34" s="67"/>
+      <c r="D34" s="67"/>
+      <c r="E34" s="67"/>
+      <c r="F34" s="67"/>
+      <c r="G34" s="68"/>
+    </row>
+    <row r="35" spans="1:7">
+      <c r="A35" s="55" t="s">
+        <v>1</v>
+      </c>
+      <c r="B35" s="52" t="s">
+        <v>2</v>
+      </c>
+      <c r="C35" s="52" t="s">
+        <v>3</v>
+      </c>
+      <c r="D35" s="53" t="s">
+        <v>4</v>
+      </c>
+      <c r="E35" s="54" t="s">
+        <v>5</v>
+      </c>
+      <c r="F35" s="53" t="s">
+        <v>6</v>
+      </c>
+      <c r="G35" s="56" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" ht="30.75">
+      <c r="A36" s="42" t="s">
+        <v>65</v>
+      </c>
+      <c r="B36" s="23">
+        <v>3</v>
+      </c>
+      <c r="C36" s="52"/>
+      <c r="D36" s="22" t="s">
+        <v>86</v>
+      </c>
+      <c r="E36" s="54"/>
+      <c r="F36" s="53"/>
+      <c r="G36" s="56"/>
+    </row>
+    <row r="37" spans="1:7" ht="30.75">
+      <c r="A37" s="42" t="s">
+        <v>69</v>
+      </c>
+      <c r="B37" s="23">
+        <v>3</v>
+      </c>
+      <c r="C37" s="19"/>
+      <c r="D37" s="21" t="s">
+        <v>87</v>
+      </c>
+      <c r="E37" s="18"/>
+      <c r="F37" s="21"/>
+      <c r="G37" s="43"/>
+    </row>
+    <row r="38" spans="1:7" ht="30.75">
+      <c r="A38" s="42" t="s">
+        <v>73</v>
+      </c>
+      <c r="B38" s="23">
+        <v>3</v>
+      </c>
+      <c r="C38" s="23"/>
+      <c r="D38" s="21" t="s">
+        <v>88</v>
+      </c>
+      <c r="E38" s="19"/>
+      <c r="F38" s="20"/>
+      <c r="G38" s="43"/>
+    </row>
+    <row r="39" spans="1:7" ht="30.75">
+      <c r="A39" s="42" t="s">
+        <v>76</v>
+      </c>
+      <c r="B39" s="23">
+        <v>3</v>
+      </c>
+      <c r="C39" s="19"/>
+      <c r="D39" s="21" t="s">
+        <v>89</v>
+      </c>
+      <c r="E39" s="18"/>
+      <c r="F39" s="21"/>
+      <c r="G39" s="43"/>
+    </row>
+    <row r="40" spans="1:7" ht="30.75">
+      <c r="A40" s="42" t="s">
+        <v>82</v>
+      </c>
+      <c r="B40" s="23">
+        <v>3</v>
+      </c>
+      <c r="C40" s="19"/>
+      <c r="D40" s="20" t="s">
+        <v>90</v>
+      </c>
+      <c r="E40" s="18"/>
+      <c r="F40" s="21"/>
+      <c r="G40" s="43"/>
+    </row>
+    <row r="41" spans="1:7">
+      <c r="A41" s="42" t="s">
+        <v>91</v>
+      </c>
+      <c r="B41" s="63">
+        <v>3</v>
+      </c>
+      <c r="C41" s="23"/>
+      <c r="D41" s="22" t="s">
+        <v>92</v>
+      </c>
+      <c r="E41" s="18"/>
+      <c r="F41" s="21"/>
+      <c r="G41" s="43"/>
+    </row>
+    <row r="42" spans="1:7" ht="30.75">
+      <c r="A42" s="61" t="s">
+        <v>93</v>
+      </c>
+      <c r="B42" s="57">
+        <v>3</v>
+      </c>
+      <c r="C42" s="62"/>
+      <c r="D42" s="58" t="s">
+        <v>94</v>
+      </c>
+      <c r="E42" s="59"/>
+      <c r="F42" s="51"/>
+      <c r="G42" s="60"/>
+    </row>
+    <row r="43" spans="1:7">
+      <c r="A43" s="69"/>
+      <c r="B43" s="69"/>
+      <c r="C43" s="69"/>
+      <c r="D43" s="69"/>
+      <c r="E43" s="69"/>
+      <c r="F43" s="69"/>
+      <c r="G43" s="69"/>
+    </row>
+    <row r="44" spans="1:7">
+      <c r="A44" s="70"/>
+      <c r="B44" s="70"/>
+      <c r="C44" s="70"/>
+      <c r="D44" s="70"/>
+      <c r="E44" s="70"/>
+      <c r="F44" s="70"/>
+      <c r="G44" s="70"/>
+    </row>
+    <row r="45" spans="1:7">
+      <c r="A45" s="70"/>
+      <c r="B45" s="70"/>
+      <c r="C45" s="70"/>
+      <c r="D45" s="70"/>
+      <c r="E45" s="70"/>
+      <c r="F45" s="70"/>
+      <c r="G45" s="70"/>
+    </row>
+    <row r="46" spans="1:7">
+      <c r="A46" s="70"/>
+      <c r="B46" s="70"/>
+      <c r="C46" s="70"/>
+      <c r="D46" s="70"/>
+      <c r="E46" s="70"/>
+      <c r="F46" s="70"/>
+      <c r="G46" s="70"/>
+    </row>
+    <row r="47" spans="1:7">
+      <c r="A47" s="70"/>
+      <c r="B47" s="70"/>
+      <c r="C47" s="70"/>
+      <c r="D47" s="70"/>
+      <c r="E47" s="70"/>
+      <c r="F47" s="70"/>
+      <c r="G47" s="70"/>
+    </row>
+    <row r="48" spans="1:7">
+      <c r="A48" s="70"/>
+      <c r="B48" s="70"/>
+      <c r="C48" s="70"/>
+      <c r="D48" s="70"/>
+      <c r="E48" s="70"/>
+      <c r="F48" s="70"/>
+      <c r="G48" s="70"/>
+    </row>
+    <row r="49" spans="1:7" ht="46.5">
+      <c r="A49" s="66" t="s">
+        <v>0</v>
+      </c>
+      <c r="B49" s="67"/>
+      <c r="C49" s="67"/>
+      <c r="D49" s="67"/>
+      <c r="E49" s="67"/>
+      <c r="F49" s="67"/>
+      <c r="G49" s="68"/>
+    </row>
+    <row r="50" spans="1:7">
+      <c r="A50" s="55" t="s">
+        <v>1</v>
+      </c>
+      <c r="B50" s="52" t="s">
+        <v>2</v>
+      </c>
+      <c r="C50" s="52" t="s">
+        <v>3</v>
+      </c>
+      <c r="D50" s="53" t="s">
+        <v>4</v>
+      </c>
+      <c r="E50" s="54" t="s">
+        <v>5</v>
+      </c>
+      <c r="F50" s="53" t="s">
+        <v>6</v>
+      </c>
+      <c r="G50" s="56" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" ht="30.75">
+      <c r="A51" s="42" t="s">
+        <v>95</v>
+      </c>
+      <c r="B51" s="23">
+        <v>4</v>
+      </c>
+      <c r="C51" s="23"/>
+      <c r="D51" s="21" t="s">
+        <v>96</v>
+      </c>
+      <c r="E51" s="19"/>
+      <c r="F51" s="20"/>
+      <c r="G51" s="43"/>
+    </row>
+    <row r="52" spans="1:7">
+      <c r="A52" s="42" t="s">
+        <v>97</v>
+      </c>
+      <c r="B52" s="23">
+        <v>4</v>
+      </c>
+      <c r="C52" s="19"/>
+      <c r="D52" s="21" t="s">
+        <v>98</v>
+      </c>
+      <c r="E52" s="19"/>
+      <c r="F52" s="20"/>
+      <c r="G52" s="43"/>
+    </row>
+    <row r="53" spans="1:7" ht="30.75">
+      <c r="A53" s="42" t="s">
+        <v>99</v>
+      </c>
+      <c r="B53" s="23">
+        <v>4</v>
+      </c>
+      <c r="C53" s="19"/>
+      <c r="D53" s="22" t="s">
+        <v>100</v>
+      </c>
+      <c r="E53" s="19"/>
+      <c r="F53" s="20"/>
+      <c r="G53" s="43"/>
+    </row>
+    <row r="54" spans="1:7" ht="30.75">
+      <c r="A54" s="42" t="s">
+        <v>101</v>
+      </c>
+      <c r="B54" s="23">
+        <v>4</v>
+      </c>
+      <c r="C54" s="19"/>
+      <c r="D54" s="22" t="s">
+        <v>102</v>
+      </c>
+      <c r="E54" s="19"/>
+      <c r="F54" s="20"/>
+      <c r="G54" s="43"/>
+    </row>
+    <row r="55" spans="1:7" ht="30.75">
+      <c r="A55" s="42" t="s">
+        <v>103</v>
+      </c>
+      <c r="B55" s="23">
+        <v>4</v>
+      </c>
+      <c r="C55" s="19"/>
+      <c r="D55" s="21" t="s">
+        <v>104</v>
+      </c>
+      <c r="E55" s="19"/>
+      <c r="F55" s="20"/>
+      <c r="G55" s="43"/>
+    </row>
+    <row r="56" spans="1:7" ht="30.75">
+      <c r="A56" s="42" t="s">
+        <v>105</v>
+      </c>
+      <c r="B56" s="23">
+        <v>4</v>
+      </c>
+      <c r="C56" s="19"/>
+      <c r="D56" s="21" t="s">
+        <v>106</v>
+      </c>
+      <c r="E56" s="19"/>
+      <c r="F56" s="20"/>
+      <c r="G56" s="43"/>
+    </row>
+    <row r="57" spans="1:7" ht="30.75">
+      <c r="A57" s="42" t="s">
+        <v>107</v>
+      </c>
+      <c r="B57" s="23">
+        <v>4</v>
+      </c>
+      <c r="C57" s="19"/>
+      <c r="D57" s="21" t="s">
+        <v>108</v>
+      </c>
+      <c r="E57" s="19"/>
+      <c r="F57" s="20"/>
+      <c r="G57" s="43"/>
+    </row>
+    <row r="58" spans="1:7" ht="30.75">
+      <c r="A58" s="45" t="s">
+        <v>109</v>
+      </c>
+      <c r="B58" s="57">
+        <v>4</v>
+      </c>
+      <c r="C58" s="47"/>
+      <c r="D58" s="58" t="s">
+        <v>110</v>
+      </c>
+      <c r="E58" s="47"/>
+      <c r="F58" s="48"/>
+      <c r="G58" s="60"/>
+    </row>
+    <row r="61" spans="1:7">
+      <c r="A61" s="8"/>
+      <c r="B61" s="11"/>
+      <c r="C61" s="11"/>
+    </row>
+    <row r="62" spans="1:7">
+      <c r="A62" s="8"/>
+      <c r="B62" s="11"/>
+      <c r="C62" s="11"/>
+    </row>
+    <row r="63" spans="1:7">
+      <c r="A63" s="8"/>
+      <c r="B63" s="11"/>
+    </row>
+    <row r="64" spans="1:7">
+      <c r="A64" s="8"/>
+      <c r="B64" s="11"/>
+    </row>
+    <row r="65" spans="1:6">
+      <c r="A65" s="8"/>
+      <c r="B65" s="11"/>
+      <c r="C65" s="11"/>
+    </row>
+    <row r="68" spans="1:6">
+      <c r="A68" s="8"/>
+      <c r="B68" s="11"/>
+      <c r="C68" s="11"/>
+      <c r="E68" s="8"/>
+      <c r="F68" s="5"/>
+    </row>
+    <row r="69" spans="1:6">
+      <c r="A69" s="8"/>
+      <c r="B69" s="11"/>
+      <c r="C69" s="11"/>
+      <c r="E69" s="8"/>
+      <c r="F69" s="5"/>
+    </row>
+    <row r="70" spans="1:6">
+      <c r="A70" s="8"/>
+      <c r="B70" s="11"/>
+      <c r="C70" s="11"/>
+      <c r="E70" s="8"/>
+      <c r="F70" s="5"/>
+    </row>
+    <row r="71" spans="1:6">
+      <c r="A71" s="8"/>
+      <c r="B71" s="11"/>
+      <c r="C71" s="11"/>
+      <c r="E71" s="8"/>
+      <c r="F71" s="5"/>
+    </row>
+    <row r="72" spans="1:6">
+      <c r="A72" s="8"/>
+      <c r="B72" s="11"/>
+      <c r="C72" s="11"/>
+      <c r="D72" s="5"/>
+      <c r="E72" s="8"/>
+      <c r="F72" s="5"/>
+    </row>
+  </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="A49:G49"/>
+    <mergeCell ref="A43:G48"/>
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A12:G12"/>
+    <mergeCell ref="A7:G11"/>
+    <mergeCell ref="A34:G34"/>
+    <mergeCell ref="A26:G33"/>
+  </mergeCells>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9CB832A2-D8FF-4CDB-9EA2-608A7EB2BB39}">
   <dimension ref="A1:G25"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="13.42578125" customWidth="1"/>
     <col min="2" max="2" width="6" customWidth="1"/>
@@ -1027,18 +2411,18 @@
     <col min="7" max="7" width="32.28515625" style="6" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="46.5" x14ac:dyDescent="0.7">
-      <c r="A1" s="36" t="s">
+    <row r="1" spans="1:7" ht="46.5">
+      <c r="A1" s="78" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="36"/>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
-      <c r="E1" s="36"/>
-      <c r="F1" s="36"/>
-      <c r="G1" s="36"/>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B1" s="78"/>
+      <c r="C1" s="78"/>
+      <c r="D1" s="78"/>
+      <c r="E1" s="78"/>
+      <c r="F1" s="78"/>
+      <c r="G1" s="78"/>
+    </row>
+    <row r="2" spans="1:7">
       <c r="A2" s="15" t="s">
         <v>1</v>
       </c>
@@ -1061,7 +2445,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="76.5">
       <c r="A3" s="4" t="s">
         <v>8</v>
       </c>
@@ -1084,7 +2468,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="76.5">
       <c r="A4" s="4" t="s">
         <v>14</v>
       </c>
@@ -1107,7 +2491,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="76.5">
       <c r="A5" s="4" t="s">
         <v>20</v>
       </c>
@@ -1130,7 +2514,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="159" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="159" customHeight="1">
       <c r="A6" s="12" t="s">
         <v>26</v>
       </c>
@@ -1150,10 +2534,10 @@
         <v>30</v>
       </c>
       <c r="G6" s="14" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="51" customHeight="1" x14ac:dyDescent="0.25">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="51" customHeight="1">
       <c r="A7" s="8"/>
       <c r="B7" s="11"/>
       <c r="C7" s="11"/>
@@ -1162,7 +2546,7 @@
       <c r="F7" s="9"/>
       <c r="G7" s="5"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7">
       <c r="A8" s="8"/>
       <c r="B8" s="11"/>
       <c r="C8" s="11"/>
@@ -1171,7 +2555,7 @@
       <c r="F8" s="5"/>
       <c r="G8" s="5"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7">
       <c r="A9" s="8"/>
       <c r="B9" s="11"/>
       <c r="C9" s="11"/>
@@ -1180,7 +2564,7 @@
       <c r="F9" s="5"/>
       <c r="G9" s="5"/>
     </row>
-    <row r="10" spans="1:7" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" ht="38.25" customHeight="1">
       <c r="A10" s="8"/>
       <c r="B10" s="11"/>
       <c r="C10" s="11"/>
@@ -1189,7 +2573,7 @@
       <c r="F10" s="5"/>
       <c r="G10" s="5"/>
     </row>
-    <row r="11" spans="1:7" ht="51" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" ht="51" customHeight="1">
       <c r="A11" s="8"/>
       <c r="B11" s="11"/>
       <c r="C11" s="11"/>
@@ -1198,7 +2582,7 @@
       <c r="F11" s="9"/>
       <c r="G11" s="5"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7">
       <c r="A12" s="8"/>
       <c r="B12" s="11"/>
       <c r="C12" s="11"/>
@@ -1207,7 +2591,7 @@
       <c r="F12" s="5"/>
       <c r="G12" s="5"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7">
       <c r="A13" s="8"/>
       <c r="B13" s="11"/>
       <c r="C13" s="11"/>
@@ -1216,7 +2600,7 @@
       <c r="F13" s="5"/>
       <c r="G13" s="5"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7">
       <c r="A14" s="8"/>
       <c r="B14" s="11"/>
       <c r="C14" s="11"/>
@@ -1225,7 +2609,7 @@
       <c r="F14" s="5"/>
       <c r="G14" s="5"/>
     </row>
-    <row r="15" spans="1:7" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" ht="38.25" customHeight="1">
       <c r="A15" s="8"/>
       <c r="B15" s="11"/>
       <c r="C15" s="11"/>
@@ -1234,7 +2618,7 @@
       <c r="F15" s="5"/>
       <c r="G15" s="5"/>
     </row>
-    <row r="16" spans="1:7" ht="51" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" ht="51" customHeight="1">
       <c r="A16" s="8"/>
       <c r="B16" s="11"/>
       <c r="C16" s="11"/>
@@ -1243,7 +2627,7 @@
       <c r="F16" s="9"/>
       <c r="G16" s="5"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7">
       <c r="A17" s="8"/>
       <c r="B17" s="11"/>
       <c r="C17" s="11"/>
@@ -1252,7 +2636,7 @@
       <c r="F17" s="5"/>
       <c r="G17" s="5"/>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7">
       <c r="A18" s="8"/>
       <c r="B18" s="11"/>
       <c r="C18" s="11"/>
@@ -1261,7 +2645,7 @@
       <c r="F18" s="5"/>
       <c r="G18" s="5"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7">
       <c r="A19" s="8"/>
       <c r="B19" s="11"/>
       <c r="C19" s="11"/>
@@ -1270,7 +2654,7 @@
       <c r="F19" s="5"/>
       <c r="G19" s="5"/>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7">
       <c r="A20" s="8"/>
       <c r="B20" s="11"/>
       <c r="C20" s="11"/>
@@ -1279,7 +2663,7 @@
       <c r="F20" s="5"/>
       <c r="G20" s="5"/>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7">
       <c r="A21" s="8"/>
       <c r="B21" s="11"/>
       <c r="C21" s="11"/>
@@ -1288,7 +2672,7 @@
       <c r="F21" s="5"/>
       <c r="G21" s="5"/>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7">
       <c r="A22" s="8"/>
       <c r="B22" s="11"/>
       <c r="C22" s="11"/>
@@ -1297,19 +2681,19 @@
       <c r="F22" s="5"/>
       <c r="G22" s="5"/>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7">
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
       <c r="E23" s="7"/>
       <c r="F23" s="10"/>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7">
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
       <c r="E24" s="2"/>
       <c r="F24" s="10"/>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7">
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
       <c r="F25" s="10"/>
@@ -1324,306 +2708,326 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5CE71AD-9C29-4F4C-8F29-96BDEAFA29E4}">
-  <dimension ref="A1:G13"/>
+  <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14:G14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="16.7109375" customWidth="1"/>
     <col min="2" max="2" width="7.85546875" customWidth="1"/>
     <col min="3" max="3" width="20" customWidth="1"/>
-    <col min="4" max="4" width="80.5703125" customWidth="1"/>
+    <col min="4" max="4" width="72.140625" customWidth="1"/>
     <col min="5" max="5" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="53.85546875" customWidth="1"/>
-    <col min="7" max="7" width="60.5703125" customWidth="1"/>
+    <col min="6" max="6" width="39" customWidth="1"/>
+    <col min="7" max="7" width="39.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="46.5" x14ac:dyDescent="0.7">
-      <c r="A1" s="37" t="s">
+    <row r="1" spans="1:7" ht="46.5">
+      <c r="A1" s="72" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="38"/>
-      <c r="C1" s="38"/>
-      <c r="D1" s="38"/>
-      <c r="E1" s="38"/>
-      <c r="F1" s="38"/>
-      <c r="G1" s="39"/>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="22" t="s">
+      <c r="B1" s="73"/>
+      <c r="C1" s="73"/>
+      <c r="D1" s="73"/>
+      <c r="E1" s="73"/>
+      <c r="F1" s="73"/>
+      <c r="G1" s="74"/>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="23" t="s">
+      <c r="B2" s="38" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="23" t="s">
+      <c r="C2" s="38" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="24" t="s">
+      <c r="D2" s="39" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="25" t="s">
+      <c r="E2" s="40" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="24" t="s">
+      <c r="F2" s="39" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="26" t="s">
+      <c r="G2" s="41" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="94.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="27" t="s">
-        <v>31</v>
-      </c>
-      <c r="B3" s="21">
+    <row r="3" spans="1:7" ht="121.5">
+      <c r="A3" s="42" t="s">
+        <v>32</v>
+      </c>
+      <c r="B3" s="36">
         <v>2</v>
       </c>
-      <c r="C3" s="19" t="s">
-        <v>32</v>
-      </c>
-      <c r="D3" s="31" t="s">
+      <c r="C3" s="23" t="s">
         <v>33</v>
       </c>
-      <c r="E3" s="32" t="s">
+      <c r="D3" s="50" t="s">
+        <v>34</v>
+      </c>
+      <c r="E3" s="54" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="18" t="s">
-        <v>34</v>
-      </c>
-      <c r="G3" s="28" t="s">
+      <c r="F3" s="21" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" ht="67.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="27" t="s">
+      <c r="G3" s="44" t="s">
         <v>36</v>
       </c>
-      <c r="B4" s="21">
+    </row>
+    <row r="4" spans="1:7" ht="67.5" customHeight="1">
+      <c r="A4" s="42" t="s">
+        <v>37</v>
+      </c>
+      <c r="B4" s="36">
         <v>2</v>
       </c>
-      <c r="C4" s="19" t="s">
-        <v>37</v>
-      </c>
-      <c r="D4" s="18" t="s">
+      <c r="C4" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="E4" s="32" t="s">
+      <c r="D4" s="21" t="s">
         <v>39</v>
       </c>
-      <c r="F4" s="18" t="s">
+      <c r="E4" s="54" t="s">
         <v>40</v>
       </c>
-      <c r="G4" s="28" t="s">
+      <c r="F4" s="21" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" ht="85.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="27" t="s">
+      <c r="G4" s="44" t="s">
         <v>42</v>
       </c>
-      <c r="B5" s="21">
+    </row>
+    <row r="5" spans="1:7" ht="106.5">
+      <c r="A5" s="42" t="s">
+        <v>43</v>
+      </c>
+      <c r="B5" s="36">
         <v>2</v>
       </c>
-      <c r="C5" s="19" t="s">
-        <v>43</v>
-      </c>
-      <c r="D5" s="18" t="s">
+      <c r="C5" s="23" t="s">
         <v>44</v>
       </c>
-      <c r="E5" s="32" t="s">
+      <c r="D5" s="21" t="s">
         <v>45</v>
       </c>
-      <c r="F5" s="18" t="s">
+      <c r="E5" s="54" t="s">
         <v>46</v>
       </c>
-      <c r="G5" s="28" t="s">
+      <c r="F5" s="21" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" ht="70.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="27" t="s">
+      <c r="G5" s="44" t="s">
         <v>48</v>
       </c>
-      <c r="B6" s="21"/>
+    </row>
+    <row r="6" spans="1:7" ht="76.5">
+      <c r="A6" s="42" t="s">
+        <v>49</v>
+      </c>
+      <c r="B6" s="36"/>
       <c r="C6" s="1" t="s">
         <v>9</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="E6" s="32" t="s">
         <v>50</v>
+      </c>
+      <c r="E6" s="54" t="s">
+        <v>51</v>
       </c>
       <c r="F6" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="G6" s="20" t="s">
+      <c r="G6" s="25" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="70.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="27" t="s">
-        <v>51</v>
-      </c>
-      <c r="B7" s="21"/>
+    <row r="7" spans="1:7" ht="76.5">
+      <c r="A7" s="42" t="s">
+        <v>52</v>
+      </c>
+      <c r="B7" s="36"/>
       <c r="C7" s="1" t="s">
         <v>15</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="E7" s="32" t="s">
-        <v>50</v>
+        <v>53</v>
+      </c>
+      <c r="E7" s="54" t="s">
+        <v>51</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="G7" s="20" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" ht="75.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="27" t="s">
+      <c r="G7" s="25" t="s">
         <v>55</v>
       </c>
-      <c r="B8" s="21">
+    </row>
+    <row r="8" spans="1:7" ht="76.5">
+      <c r="A8" s="42" t="s">
+        <v>56</v>
+      </c>
+      <c r="B8" s="36">
         <v>2</v>
       </c>
-      <c r="C8" s="19" t="s">
-        <v>43</v>
-      </c>
-      <c r="D8" s="18" t="s">
-        <v>56</v>
-      </c>
-      <c r="E8" s="32" t="s">
-        <v>45</v>
-      </c>
-      <c r="F8" s="18" t="s">
+      <c r="C8" s="23" t="s">
+        <v>44</v>
+      </c>
+      <c r="D8" s="21" t="s">
         <v>57</v>
       </c>
-      <c r="G8" s="28" t="s">
+      <c r="E8" s="54" t="s">
+        <v>46</v>
+      </c>
+      <c r="F8" s="21" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" ht="75.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="27" t="s">
+      <c r="G8" s="44" t="s">
         <v>59</v>
       </c>
-      <c r="B9" s="21">
+    </row>
+    <row r="9" spans="1:7" ht="91.5">
+      <c r="A9" s="42" t="s">
+        <v>60</v>
+      </c>
+      <c r="B9" s="36">
         <v>2</v>
       </c>
-      <c r="C9" s="19" t="s">
-        <v>43</v>
-      </c>
-      <c r="D9" s="18" t="s">
-        <v>60</v>
-      </c>
-      <c r="E9" s="32" t="s">
+      <c r="C9" s="23" t="s">
+        <v>44</v>
+      </c>
+      <c r="D9" s="21" t="s">
         <v>61</v>
       </c>
-      <c r="F9" s="18" t="s">
+      <c r="E9" s="54" t="s">
         <v>62</v>
       </c>
-      <c r="G9" s="28" t="s">
+      <c r="F9" s="21" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" ht="75.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="27" t="s">
-        <v>64</v>
-      </c>
-      <c r="B10" s="21">
+      <c r="G9" s="44" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="91.5">
+      <c r="A10" s="42" t="s">
+        <v>65</v>
+      </c>
+      <c r="B10" s="36">
         <v>2</v>
       </c>
-      <c r="C10" s="19" t="s">
-        <v>43</v>
-      </c>
-      <c r="D10" s="18" t="s">
-        <v>65</v>
-      </c>
-      <c r="E10" s="32" t="s">
-        <v>61</v>
-      </c>
-      <c r="F10" s="18" t="s">
+      <c r="C10" s="23" t="s">
+        <v>44</v>
+      </c>
+      <c r="D10" s="21" t="s">
         <v>66</v>
       </c>
-      <c r="G10" s="28" t="s">
+      <c r="E10" s="54" t="s">
+        <v>62</v>
+      </c>
+      <c r="F10" s="21" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A11" s="27" t="s">
-        <v>68</v>
-      </c>
-      <c r="B11" s="21">
+      <c r="G10" s="44" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="60.75">
+      <c r="A11" s="42" t="s">
+        <v>69</v>
+      </c>
+      <c r="B11" s="36">
         <v>2</v>
       </c>
-      <c r="C11" s="19" t="s">
-        <v>43</v>
-      </c>
-      <c r="D11" s="18" t="s">
-        <v>69</v>
-      </c>
-      <c r="E11" s="32" t="s">
+      <c r="C11" s="23" t="s">
+        <v>44</v>
+      </c>
+      <c r="D11" s="21" t="s">
+        <v>70</v>
+      </c>
+      <c r="E11" s="54" t="s">
         <v>23</v>
       </c>
-      <c r="F11" s="18" t="s">
-        <v>70</v>
-      </c>
-      <c r="G11" s="28" t="s">
+      <c r="F11" s="21" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A12" s="27" t="s">
+      <c r="G11" s="44" t="s">
         <v>72</v>
       </c>
-      <c r="B12" s="21">
+    </row>
+    <row r="12" spans="1:7" ht="60.75">
+      <c r="A12" s="42" t="s">
+        <v>73</v>
+      </c>
+      <c r="B12" s="36">
         <v>2</v>
       </c>
-      <c r="C12" s="19" t="s">
-        <v>43</v>
-      </c>
-      <c r="D12" s="18" t="s">
-        <v>73</v>
-      </c>
-      <c r="E12" s="32" t="s">
+      <c r="C12" s="23" t="s">
+        <v>44</v>
+      </c>
+      <c r="D12" s="21" t="s">
+        <v>74</v>
+      </c>
+      <c r="E12" s="54" t="s">
         <v>23</v>
       </c>
-      <c r="F12" s="18" t="s">
-        <v>74</v>
-      </c>
-      <c r="G12" s="28" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="51" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="27" t="s">
+      <c r="F12" s="21" t="s">
         <v>75</v>
       </c>
-      <c r="B13" s="29">
+      <c r="G12" s="44" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="60.75">
+      <c r="A13" s="42" t="s">
+        <v>76</v>
+      </c>
+      <c r="B13" s="46">
         <v>2</v>
       </c>
-      <c r="C13" s="33" t="s">
-        <v>76</v>
-      </c>
-      <c r="D13" s="34" t="s">
+      <c r="C13" s="57" t="s">
         <v>77</v>
       </c>
-      <c r="E13" s="35" t="s">
+      <c r="D13" s="58" t="s">
         <v>78</v>
       </c>
-      <c r="F13" s="34" t="s">
+      <c r="E13" s="64" t="s">
         <v>79</v>
       </c>
-      <c r="G13" s="30" t="s">
+      <c r="F13" s="58" t="s">
         <v>80</v>
+      </c>
+      <c r="G13" s="49" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="91.5">
+      <c r="A14" s="42" t="s">
+        <v>82</v>
+      </c>
+      <c r="B14" s="46">
+        <v>2</v>
+      </c>
+      <c r="C14" s="57"/>
+      <c r="D14" s="65" t="s">
+        <v>83</v>
+      </c>
+      <c r="E14" s="64" t="s">
+        <v>51</v>
+      </c>
+      <c r="F14" s="58" t="s">
+        <v>84</v>
+      </c>
+      <c r="G14" s="49" t="s">
+        <v>85</v>
       </c>
     </row>
   </sheetData>
@@ -1631,11 +3035,19 @@
     <mergeCell ref="A1:G1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100F6E35812089B734D91EAA291CBA3AAB8" ma:contentTypeVersion="2" ma:contentTypeDescription="Crie um novo documento." ma:contentTypeScope="" ma:versionID="eddbe7b98ac95aed3373f45f7c513afb">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="2cf9187d-8d26-48aa-b51a-02fd7482876d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="fd71642a5a878ea03ec62200d09b34f1" ns2:_="">
     <xsd:import namespace="2cf9187d-8d26-48aa-b51a-02fd7482876d"/>
@@ -1767,59 +3179,20 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
 </p:properties>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{060E6BB9-F718-47EC-A29F-E6123F084C31}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="2cf9187d-8d26-48aa-b51a-02fd7482876d"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{25BB1E34-FD9F-4ECD-ADE5-D5736D8FE27A}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{41C642EC-9D65-4F75-8CF9-10B937343010}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="2cf9187d-8d26-48aa-b51a-02fd7482876d"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{060E6BB9-F718-47EC-A29F-E6123F084C31}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{25BB1E34-FD9F-4ECD-ADE5-D5736D8FE27A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{41C642EC-9D65-4F75-8CF9-10B937343010}"/>
 </file>
</xml_diff>